<commit_message>
Adicionando estruturas e prototipo do site
</commit_message>
<xml_diff>
--- a/DOCUMENTOS/backlog.xlsx
+++ b/DOCUMENTOS/backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\playk\OneDrive\Área de Trabalho\Projeto individual\projetoIndividual\DOCUMENTOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/10a1ccb1afc08725/Área de Trabalho/Projeto individual/projetoIndividual/DOCUMENTOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ADB2838-BC6D-4735-B17A-5B3FC3921690}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{5C0D772D-BC51-4A43-8B57-135C898D57FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EBD020B4-5CD7-4A39-BA60-7CE8667CD9E2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Igor Sérgio RA:02211030</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -149,6 +152,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -520,15 +530,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386FE109-A2A6-4B05-93B4-E2082710041F}">
-  <dimension ref="B2:K9"/>
+  <dimension ref="B2:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
@@ -573,7 +583,9 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="4">
+        <v>44340</v>
+      </c>
     </row>
     <row r="4" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -591,7 +603,9 @@
       <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="4">
+        <v>44340</v>
+      </c>
     </row>
     <row r="5" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -609,7 +623,9 @@
       <c r="F5" s="1">
         <v>3</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="4">
+        <v>44340</v>
+      </c>
     </row>
     <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -627,7 +643,9 @@
       <c r="F6" s="1">
         <v>4</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="4">
+        <v>44340</v>
+      </c>
       <c r="K6" t="s">
         <v>16</v>
       </c>
@@ -648,7 +666,9 @@
       <c r="F7" s="1">
         <v>5</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="4">
+        <v>44340</v>
+      </c>
     </row>
     <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -666,7 +686,9 @@
       <c r="F8" s="1">
         <v>6</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="4">
+        <v>44340</v>
+      </c>
     </row>
     <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -684,7 +706,21 @@
       <c r="F9" s="1">
         <v>7</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="4">
+        <v>44340</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6">
+        <v>60</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>